<commit_message>
T-test table added to DSSR paper.
</commit_message>
<xml_diff>
--- a/papers/ISSTA_DSSR/60classes.xlsx
+++ b/papers/ISSTA_DSSR/60classes.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22220"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-440" windowWidth="25600" windowHeight="20480" tabRatio="863" firstSheet="46" activeTab="59"/>
+    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="22020" tabRatio="863" firstSheet="54" activeTab="60"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -68,7 +68,7 @@
     <sheet name="Sheet59" sheetId="59" r:id="rId59"/>
     <sheet name="Sheet60" sheetId="60" r:id="rId60"/>
     <sheet name="T-test results" sheetId="75" r:id="rId61"/>
-    <sheet name="Sheet63" sheetId="63" r:id="rId62"/>
+    <sheet name="as in paper" sheetId="77" r:id="rId62"/>
     <sheet name="Sheet64" sheetId="64" r:id="rId63"/>
     <sheet name="Sheet65" sheetId="65" r:id="rId64"/>
     <sheet name="Sheet66" sheetId="66" r:id="rId65"/>
@@ -77,6 +77,7 @@
     <sheet name="Sheet69" sheetId="69" r:id="rId68"/>
     <sheet name="Sheet70" sheetId="70" r:id="rId69"/>
     <sheet name="Sheet71" sheetId="71" r:id="rId70"/>
+    <sheet name="Sheet61" sheetId="76" r:id="rId71"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -88,7 +89,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2527" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2565" uniqueCount="134">
   <si>
     <t>org.antlr.grammar.v3.ActionTranslator</t>
   </si>
@@ -420,9 +421,6 @@
     <t>Status</t>
   </si>
   <si>
-    <t>Hibernate</t>
-  </si>
-  <si>
     <t>StringUtils</t>
   </si>
   <si>
@@ -446,6 +444,54 @@
   <si>
     <t>Xobject</t>
   </si>
+  <si>
+    <t>DSSR better</t>
+  </si>
+  <si>
+    <t>DSSR=R+&gt;R</t>
+  </si>
+  <si>
+    <t>StringHelper</t>
+  </si>
+  <si>
+    <t>DSSR=R&gt;R+</t>
+  </si>
+  <si>
+    <t>classes where DSSR is significantly better than both R+ and R</t>
+  </si>
+  <si>
+    <t>classes where DSSR and R are significantly better than R+</t>
+  </si>
+  <si>
+    <t>classes where DSSR and R+ are significantly better than R</t>
+  </si>
+  <si>
+    <t>classes where R and R+ are similar and significantly better than DSSR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S. No </t>
+  </si>
+  <si>
+    <t>ClassName</t>
+  </si>
+  <si>
+    <t>LOC</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>R+</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>R. Std</t>
+  </si>
 </sst>
 </file>
 
@@ -457,7 +503,7 @@
     <numFmt numFmtId="166" formatCode="0.00000000"/>
     <numFmt numFmtId="167" formatCode="0.000000000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -501,8 +547,13 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -545,6 +596,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -555,7 +624,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="301">
+  <cellStyleXfs count="321">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -857,8 +926,28 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -883,8 +972,21 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="301">
+  <cellStyles count="321">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1035,6 +1137,16 @@
     <cellStyle name="Followed Hyperlink" xfId="296" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="298" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="300" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="302" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="304" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="306" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="308" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="310" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="312" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="314" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="316" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="318" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="320" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1185,6 +1297,16 @@
     <cellStyle name="Hyperlink" xfId="295" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="297" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="299" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="301" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="303" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="305" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="307" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="309" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="311" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="313" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="315" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="317" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="319" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -20080,7 +20202,7 @@
   <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D31"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -20644,7 +20766,7 @@
   </sheetPr>
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
@@ -33019,7 +33141,7 @@
   </sheetPr>
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
@@ -33576,10 +33698,10 @@
 
 <file path=xl/worksheets/sheet61.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:L61"/>
+  <dimension ref="B1:L66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G64" sqref="G64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -33619,7 +33741,7 @@
       <c r="B3" s="15">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="16" t="s">
         <v>1</v>
       </c>
       <c r="D3">
@@ -33636,7 +33758,7 @@
       <c r="B4" s="15">
         <v>3</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="16" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="16">
@@ -33669,7 +33791,7 @@
       <c r="B7" s="15">
         <v>6</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="16" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="16">
@@ -33681,12 +33803,15 @@
       <c r="F7" s="17">
         <v>0.44</v>
       </c>
+      <c r="G7" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="8" spans="2:12">
       <c r="B8" s="15">
         <v>7</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="16" t="s">
         <v>6</v>
       </c>
       <c r="D8" s="16">
@@ -33709,7 +33834,7 @@
       <c r="B9" s="15">
         <v>8</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="16" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="16">
@@ -33720,6 +33845,9 @@
       </c>
       <c r="F9">
         <v>0.43</v>
+      </c>
+      <c r="G9" t="s">
+        <v>118</v>
       </c>
       <c r="I9" s="19"/>
       <c r="J9" s="19"/>
@@ -33742,7 +33870,7 @@
       <c r="B11" s="15">
         <v>10</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="16" t="s">
         <v>83</v>
       </c>
       <c r="D11" s="16">
@@ -33771,7 +33899,7 @@
       <c r="B13" s="15">
         <v>12</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="16" t="s">
         <v>11</v>
       </c>
       <c r="D13" s="16">
@@ -33834,7 +33962,7 @@
       <c r="B18" s="15">
         <v>17</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="16" t="s">
         <v>90</v>
       </c>
       <c r="D18">
@@ -33881,7 +34009,7 @@
       <c r="B21" s="15">
         <v>20</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="16" t="s">
         <v>94</v>
       </c>
       <c r="D21">
@@ -33892,6 +34020,9 @@
       </c>
       <c r="F21" s="16">
         <v>0.04</v>
+      </c>
+      <c r="G21" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="22" spans="2:12">
@@ -33906,7 +34037,7 @@
       <c r="B23" s="15">
         <v>22</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="16" t="s">
         <v>21</v>
       </c>
       <c r="D23" s="16">
@@ -33917,6 +34048,9 @@
       </c>
       <c r="F23">
         <v>0.61</v>
+      </c>
+      <c r="G23" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="24" spans="2:12">
@@ -33964,7 +34098,7 @@
       <c r="B28" s="15">
         <v>27</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="16" t="s">
         <v>26</v>
       </c>
       <c r="D28" s="16">
@@ -33973,8 +34107,11 @@
       <c r="E28">
         <v>0.56999999999999995</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="16">
         <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="G28" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="29" spans="2:12">
@@ -33998,7 +34135,7 @@
       <c r="B30" s="15">
         <v>29</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="16" t="s">
         <v>29</v>
       </c>
       <c r="D30" s="16">
@@ -34009,6 +34146,9 @@
       </c>
       <c r="F30" s="16">
         <v>0</v>
+      </c>
+      <c r="G30" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="31" spans="2:12">
@@ -34023,7 +34163,7 @@
       <c r="B32" s="15">
         <v>31</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="16" t="s">
         <v>30</v>
       </c>
       <c r="D32">
@@ -34035,12 +34175,15 @@
       <c r="F32" s="16">
         <v>0.06</v>
       </c>
-    </row>
-    <row r="33" spans="2:6">
+      <c r="G32" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7">
       <c r="B33" s="15">
         <v>32</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="16" t="s">
         <v>31</v>
       </c>
       <c r="D33" s="16">
@@ -34053,7 +34196,7 @@
         <v>0.26</v>
       </c>
     </row>
-    <row r="34" spans="2:6">
+    <row r="34" spans="2:7">
       <c r="B34" s="15">
         <v>33</v>
       </c>
@@ -34061,7 +34204,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="35" spans="2:6">
+    <row r="35" spans="2:7">
       <c r="B35" s="15">
         <v>34</v>
       </c>
@@ -34069,7 +34212,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="36" spans="2:6">
+    <row r="36" spans="2:7">
       <c r="B36" s="15">
         <v>35</v>
       </c>
@@ -34077,11 +34220,11 @@
         <v>102</v>
       </c>
     </row>
-    <row r="37" spans="2:6">
+    <row r="37" spans="2:7">
       <c r="B37" s="15">
         <v>36</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="16" t="s">
         <v>35</v>
       </c>
       <c r="D37" s="16">
@@ -34093,12 +34236,15 @@
       <c r="F37">
         <v>0.65</v>
       </c>
-    </row>
-    <row r="38" spans="2:6">
+      <c r="G37" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7">
       <c r="B38" s="15">
         <v>37</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="16" t="s">
         <v>36</v>
       </c>
       <c r="D38" s="16">
@@ -34110,8 +34256,11 @@
       <c r="F38" s="16">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="2:6">
+      <c r="G38" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7">
       <c r="B39" s="15">
         <v>38</v>
       </c>
@@ -34119,7 +34268,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="40" spans="2:6">
+    <row r="40" spans="2:7">
       <c r="B40" s="15">
         <v>39</v>
       </c>
@@ -34127,11 +34276,11 @@
         <v>104</v>
       </c>
     </row>
-    <row r="41" spans="2:6">
+    <row r="41" spans="2:7">
       <c r="B41" s="15">
         <v>40</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="16" t="s">
         <v>71</v>
       </c>
       <c r="D41">
@@ -34143,12 +34292,15 @@
       <c r="F41" s="16">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="42" spans="2:6">
+      <c r="G41" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7">
       <c r="B42" s="15">
         <v>41</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="16" t="s">
         <v>105</v>
       </c>
       <c r="D42" s="16">
@@ -34160,8 +34312,11 @@
       <c r="F42">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="2:6">
+      <c r="G42" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7">
       <c r="B43" s="15">
         <v>42</v>
       </c>
@@ -34169,11 +34324,11 @@
         <v>106</v>
       </c>
     </row>
-    <row r="44" spans="2:6">
+    <row r="44" spans="2:7">
       <c r="B44" s="15">
         <v>43</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="16" t="s">
         <v>41</v>
       </c>
       <c r="D44" s="16">
@@ -34185,12 +34340,15 @@
       <c r="F44" s="16">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="45" spans="2:6">
+      <c r="G44" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7">
       <c r="B45" s="15">
         <v>44</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" s="16" t="s">
         <v>42</v>
       </c>
       <c r="D45" s="16">
@@ -34202,8 +34360,11 @@
       <c r="F45" s="16">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="2:6">
+      <c r="G45" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7">
       <c r="B46" s="15">
         <v>45</v>
       </c>
@@ -34211,11 +34372,11 @@
         <v>107</v>
       </c>
     </row>
-    <row r="47" spans="2:6">
+    <row r="47" spans="2:7">
       <c r="B47" s="15">
         <v>46</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C47" s="16" t="s">
         <v>108</v>
       </c>
       <c r="D47" s="16">
@@ -34227,8 +34388,11 @@
       <c r="F47" s="16">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="2:6">
+      <c r="G47" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7">
       <c r="B48" s="15">
         <v>47</v>
       </c>
@@ -34236,11 +34400,11 @@
         <v>109</v>
       </c>
     </row>
-    <row r="49" spans="2:6">
+    <row r="49" spans="2:8">
       <c r="B49" s="15">
         <v>48</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C49" s="16" t="s">
         <v>47</v>
       </c>
       <c r="D49" s="16">
@@ -34252,13 +34416,16 @@
       <c r="F49" s="16">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="2:6">
+      <c r="G49" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="50" spans="2:8">
       <c r="B50" s="15">
         <v>49</v>
       </c>
-      <c r="C50" t="s">
-        <v>110</v>
+      <c r="C50" s="16" t="s">
+        <v>120</v>
       </c>
       <c r="D50" s="16">
         <v>0.03</v>
@@ -34269,29 +34436,32 @@
       <c r="F50" s="16">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="51" spans="2:6">
+      <c r="G50" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8">
       <c r="B51" s="15">
         <v>50</v>
       </c>
       <c r="C51" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="52" spans="2:6">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="52" spans="2:8">
       <c r="B52" s="15">
         <v>51</v>
       </c>
       <c r="C52" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="53" spans="2:6">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="53" spans="2:8">
       <c r="B53" s="15">
         <v>52</v>
       </c>
       <c r="C53" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D53">
         <v>0.1</v>
@@ -34303,15 +34473,15 @@
         <v>0.47</v>
       </c>
     </row>
-    <row r="54" spans="2:6">
+    <row r="54" spans="2:8">
       <c r="B54" s="15">
         <v>53</v>
       </c>
       <c r="C54" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="55" spans="2:6">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="55" spans="2:8">
       <c r="B55" s="15">
         <v>54</v>
       </c>
@@ -34328,23 +34498,23 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="56" spans="2:6">
+    <row r="56" spans="2:8">
       <c r="B56" s="15">
         <v>55</v>
       </c>
       <c r="C56" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="57" spans="2:6">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="57" spans="2:8">
       <c r="B57" s="15">
         <v>56</v>
       </c>
       <c r="C57" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="58" spans="2:6">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="58" spans="2:8">
       <c r="B58" s="15">
         <v>57</v>
       </c>
@@ -34361,27 +34531,27 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="59" spans="2:6">
+    <row r="59" spans="2:8">
       <c r="B59" s="15">
         <v>58</v>
       </c>
       <c r="C59" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="60" spans="2:6">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="60" spans="2:8">
       <c r="B60" s="15">
         <v>59</v>
       </c>
       <c r="C60" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="61" spans="2:6">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="61" spans="2:8">
       <c r="B61" s="15">
         <v>60</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C61" s="16" t="s">
         <v>60</v>
       </c>
       <c r="D61">
@@ -34392,6 +34562,42 @@
       </c>
       <c r="F61">
         <v>0.86</v>
+      </c>
+    </row>
+    <row r="63" spans="2:8">
+      <c r="G63">
+        <v>6</v>
+      </c>
+      <c r="H63" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="64" spans="2:8">
+      <c r="D64">
+        <f>COUNT(D3:D61)</f>
+        <v>29</v>
+      </c>
+      <c r="G64">
+        <v>8</v>
+      </c>
+      <c r="H64" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="65" spans="7:8">
+      <c r="G65">
+        <v>2</v>
+      </c>
+      <c r="H65" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="66" spans="7:8">
+      <c r="G66">
+        <v>0</v>
+      </c>
+      <c r="H66" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -34401,6 +34607,7 @@
     <mergeCell ref="I18:L20"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -34411,13 +34618,2794 @@
 
 <file path=xl/worksheets/sheet62.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B2:P64"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="E10" workbookViewId="0">
+      <selection activeCell="P51" sqref="P51"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:16">
+      <c r="B2" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>127</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="E2" s="21"/>
+      <c r="F2" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="G2" s="22"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="J2" s="23"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="24"/>
+      <c r="N2" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="O2" s="23"/>
+      <c r="P2" s="24"/>
+    </row>
+    <row r="3" spans="2:16">
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="F3" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="G3" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="H3" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="I3" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="J3" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="K3" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="L3" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="M3" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="N3" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="O3" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="P3" s="24" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="4" spans="2:16">
+      <c r="B4" s="16">
+        <v>1</v>
+      </c>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16">
+        <v>709</v>
+      </c>
+      <c r="E4" s="16">
+        <v>96</v>
+      </c>
+      <c r="F4" s="16">
+        <v>96</v>
+      </c>
+      <c r="G4" s="16">
+        <v>96</v>
+      </c>
+      <c r="H4" s="16">
+        <v>0</v>
+      </c>
+      <c r="I4" s="16">
+        <v>96</v>
+      </c>
+      <c r="J4" s="16">
+        <v>96</v>
+      </c>
+      <c r="K4" s="16">
+        <v>96</v>
+      </c>
+      <c r="L4" s="16">
+        <v>0</v>
+      </c>
+      <c r="M4" s="16">
+        <v>96</v>
+      </c>
+      <c r="N4" s="16">
+        <v>96</v>
+      </c>
+      <c r="O4" s="16">
+        <v>96</v>
+      </c>
+      <c r="P4" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:16">
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>1180</v>
+      </c>
+      <c r="E5">
+        <v>80</v>
+      </c>
+      <c r="F5">
+        <v>83</v>
+      </c>
+      <c r="G5">
+        <v>79</v>
+      </c>
+      <c r="H5">
+        <v>0.02</v>
+      </c>
+      <c r="I5">
+        <v>80</v>
+      </c>
+      <c r="J5">
+        <v>83</v>
+      </c>
+      <c r="K5">
+        <v>79</v>
+      </c>
+      <c r="L5">
+        <v>0.02</v>
+      </c>
+      <c r="M5">
+        <v>80</v>
+      </c>
+      <c r="N5">
+        <v>83</v>
+      </c>
+      <c r="O5">
+        <v>79</v>
+      </c>
+      <c r="P5">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16">
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>292</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+      <c r="F6">
+        <v>4</v>
+      </c>
+      <c r="G6">
+        <v>3</v>
+      </c>
+      <c r="H6">
+        <v>0.1</v>
+      </c>
+      <c r="I6">
+        <v>3</v>
+      </c>
+      <c r="J6">
+        <v>4</v>
+      </c>
+      <c r="K6">
+        <v>3</v>
+      </c>
+      <c r="L6">
+        <v>0.13</v>
+      </c>
+      <c r="M6">
+        <v>3</v>
+      </c>
+      <c r="N6">
+        <v>4</v>
+      </c>
+      <c r="O6">
+        <v>3</v>
+      </c>
+      <c r="P6">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16">
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <v>575</v>
+      </c>
+      <c r="E7">
+        <v>9</v>
+      </c>
+      <c r="F7">
+        <v>9</v>
+      </c>
+      <c r="G7">
+        <v>9</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>9</v>
+      </c>
+      <c r="J7">
+        <v>9</v>
+      </c>
+      <c r="K7">
+        <v>9</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>9</v>
+      </c>
+      <c r="N7">
+        <v>9</v>
+      </c>
+      <c r="O7">
+        <v>9</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16">
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <v>538</v>
+      </c>
+      <c r="E8">
+        <v>7</v>
+      </c>
+      <c r="F8">
+        <v>7</v>
+      </c>
+      <c r="G8">
+        <v>7</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>7</v>
+      </c>
+      <c r="J8">
+        <v>7</v>
+      </c>
+      <c r="K8">
+        <v>7</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>7</v>
+      </c>
+      <c r="N8">
+        <v>7</v>
+      </c>
+      <c r="O8">
+        <v>7</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16">
+      <c r="B9">
+        <v>6</v>
+      </c>
+      <c r="D9">
+        <v>351</v>
+      </c>
+      <c r="E9">
+        <v>7</v>
+      </c>
+      <c r="F9">
+        <v>8</v>
+      </c>
+      <c r="G9">
+        <v>2</v>
+      </c>
+      <c r="H9">
+        <v>0.16</v>
+      </c>
+      <c r="I9">
+        <v>6</v>
+      </c>
+      <c r="J9">
+        <v>9</v>
+      </c>
+      <c r="K9">
+        <v>2</v>
+      </c>
+      <c r="L9">
+        <v>0.18</v>
+      </c>
+      <c r="M9">
+        <v>7</v>
+      </c>
+      <c r="N9">
+        <v>9</v>
+      </c>
+      <c r="O9">
+        <v>6</v>
+      </c>
+      <c r="P9">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16">
+      <c r="B10">
+        <v>7</v>
+      </c>
+      <c r="D10">
+        <v>836</v>
+      </c>
+      <c r="E10">
+        <v>4</v>
+      </c>
+      <c r="F10">
+        <v>6</v>
+      </c>
+      <c r="G10">
+        <v>4</v>
+      </c>
+      <c r="H10">
+        <v>0.13</v>
+      </c>
+      <c r="I10">
+        <v>5</v>
+      </c>
+      <c r="J10">
+        <v>6</v>
+      </c>
+      <c r="K10">
+        <v>4</v>
+      </c>
+      <c r="L10">
+        <v>0.12</v>
+      </c>
+      <c r="M10">
+        <v>5</v>
+      </c>
+      <c r="N10">
+        <v>8</v>
+      </c>
+      <c r="O10">
+        <v>4</v>
+      </c>
+      <c r="P10">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16">
+      <c r="B11">
+        <v>8</v>
+      </c>
+      <c r="D11">
+        <v>1714</v>
+      </c>
+      <c r="E11">
+        <v>33</v>
+      </c>
+      <c r="F11">
+        <v>39</v>
+      </c>
+      <c r="G11">
+        <v>20</v>
+      </c>
+      <c r="H11">
+        <v>0.1</v>
+      </c>
+      <c r="I11">
+        <v>35</v>
+      </c>
+      <c r="J11">
+        <v>38</v>
+      </c>
+      <c r="K11">
+        <v>31</v>
+      </c>
+      <c r="L11">
+        <v>0.05</v>
+      </c>
+      <c r="M11">
+        <v>36</v>
+      </c>
+      <c r="N11">
+        <v>39</v>
+      </c>
+      <c r="O11">
+        <v>32</v>
+      </c>
+      <c r="P11">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16">
+      <c r="B12">
+        <v>9</v>
+      </c>
+      <c r="D12">
+        <v>220</v>
+      </c>
+      <c r="E12">
+        <v>4</v>
+      </c>
+      <c r="F12">
+        <v>4</v>
+      </c>
+      <c r="G12">
+        <v>4</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>4</v>
+      </c>
+      <c r="J12">
+        <v>4</v>
+      </c>
+      <c r="K12">
+        <v>4</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>4</v>
+      </c>
+      <c r="N12">
+        <v>4</v>
+      </c>
+      <c r="O12">
+        <v>4</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16">
+      <c r="B13">
+        <v>10</v>
+      </c>
+      <c r="D13">
+        <v>92</v>
+      </c>
+      <c r="E13">
+        <v>7</v>
+      </c>
+      <c r="F13">
+        <v>7</v>
+      </c>
+      <c r="G13">
+        <v>3</v>
+      </c>
+      <c r="H13">
+        <v>0.19</v>
+      </c>
+      <c r="I13">
+        <v>7</v>
+      </c>
+      <c r="J13">
+        <v>7</v>
+      </c>
+      <c r="K13">
+        <v>3</v>
+      </c>
+      <c r="L13">
+        <v>0.11</v>
+      </c>
+      <c r="M13">
+        <v>7</v>
+      </c>
+      <c r="N13">
+        <v>7</v>
+      </c>
+      <c r="O13">
+        <v>7</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16">
+      <c r="B14">
+        <v>11</v>
+      </c>
+      <c r="D14">
+        <v>328</v>
+      </c>
+      <c r="E14">
+        <v>3</v>
+      </c>
+      <c r="F14">
+        <v>3</v>
+      </c>
+      <c r="G14">
+        <v>3</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>3</v>
+      </c>
+      <c r="J14">
+        <v>3</v>
+      </c>
+      <c r="K14">
+        <v>3</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>3</v>
+      </c>
+      <c r="N14">
+        <v>3</v>
+      </c>
+      <c r="O14">
+        <v>3</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16">
+      <c r="B15">
+        <v>12</v>
+      </c>
+      <c r="D15">
+        <v>675</v>
+      </c>
+      <c r="E15">
+        <v>8</v>
+      </c>
+      <c r="F15">
+        <v>9</v>
+      </c>
+      <c r="G15">
+        <v>7</v>
+      </c>
+      <c r="H15">
+        <v>0.1</v>
+      </c>
+      <c r="I15">
+        <v>8</v>
+      </c>
+      <c r="J15">
+        <v>9</v>
+      </c>
+      <c r="K15">
+        <v>7</v>
+      </c>
+      <c r="L15">
+        <v>0.1</v>
+      </c>
+      <c r="M15">
+        <v>8</v>
+      </c>
+      <c r="N15">
+        <v>9</v>
+      </c>
+      <c r="O15">
+        <v>7</v>
+      </c>
+      <c r="P15">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16">
+      <c r="B16">
+        <v>13</v>
+      </c>
+      <c r="D16">
+        <v>163</v>
+      </c>
+      <c r="E16">
+        <v>13</v>
+      </c>
+      <c r="F16">
+        <v>13</v>
+      </c>
+      <c r="G16">
+        <v>13</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>13</v>
+      </c>
+      <c r="J16">
+        <v>13</v>
+      </c>
+      <c r="K16">
+        <v>13</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>13</v>
+      </c>
+      <c r="N16">
+        <v>13</v>
+      </c>
+      <c r="O16">
+        <v>13</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:16">
+      <c r="B17">
+        <v>14</v>
+      </c>
+      <c r="D17">
+        <v>37</v>
+      </c>
+      <c r="E17">
+        <v>6</v>
+      </c>
+      <c r="F17">
+        <v>6</v>
+      </c>
+      <c r="G17">
+        <v>6</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>6</v>
+      </c>
+      <c r="J17">
+        <v>6</v>
+      </c>
+      <c r="K17">
+        <v>6</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>6</v>
+      </c>
+      <c r="N17">
+        <v>6</v>
+      </c>
+      <c r="O17">
+        <v>6</v>
+      </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16">
+      <c r="B18">
+        <v>15</v>
+      </c>
+      <c r="D18">
+        <v>3301</v>
+      </c>
+      <c r="E18">
+        <v>3</v>
+      </c>
+      <c r="F18">
+        <v>3</v>
+      </c>
+      <c r="G18">
+        <v>3</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>3</v>
+      </c>
+      <c r="J18">
+        <v>3</v>
+      </c>
+      <c r="K18">
+        <v>3</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>3</v>
+      </c>
+      <c r="N18">
+        <v>3</v>
+      </c>
+      <c r="O18">
+        <v>3</v>
+      </c>
+      <c r="P18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:16">
+      <c r="B19">
+        <v>16</v>
+      </c>
+      <c r="D19">
+        <v>83</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>1</v>
+      </c>
+      <c r="J19">
+        <v>1</v>
+      </c>
+      <c r="K19">
+        <v>1</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <v>1</v>
+      </c>
+      <c r="N19">
+        <v>1</v>
+      </c>
+      <c r="O19">
+        <v>1</v>
+      </c>
+      <c r="P19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:16">
+      <c r="B20">
+        <v>17</v>
+      </c>
+      <c r="D20">
+        <v>184</v>
+      </c>
+      <c r="E20">
+        <v>12</v>
+      </c>
+      <c r="F20">
+        <v>12</v>
+      </c>
+      <c r="G20">
+        <v>11</v>
+      </c>
+      <c r="H20">
+        <v>0.03</v>
+      </c>
+      <c r="I20">
+        <v>12</v>
+      </c>
+      <c r="J20">
+        <v>12</v>
+      </c>
+      <c r="K20">
+        <v>11</v>
+      </c>
+      <c r="L20">
+        <v>0.03</v>
+      </c>
+      <c r="M20">
+        <v>12</v>
+      </c>
+      <c r="N20">
+        <v>12</v>
+      </c>
+      <c r="O20">
+        <v>11</v>
+      </c>
+      <c r="P20">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="21" spans="2:16">
+      <c r="B21">
+        <v>18</v>
+      </c>
+      <c r="D21">
+        <v>435</v>
+      </c>
+      <c r="E21">
+        <v>5</v>
+      </c>
+      <c r="F21">
+        <v>5</v>
+      </c>
+      <c r="G21">
+        <v>5</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>5</v>
+      </c>
+      <c r="J21">
+        <v>5</v>
+      </c>
+      <c r="K21">
+        <v>5</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>5</v>
+      </c>
+      <c r="N21">
+        <v>5</v>
+      </c>
+      <c r="O21">
+        <v>5</v>
+      </c>
+      <c r="P21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:16">
+      <c r="B22">
+        <v>19</v>
+      </c>
+      <c r="D22">
+        <v>218</v>
+      </c>
+      <c r="E22">
+        <v>17</v>
+      </c>
+      <c r="F22">
+        <v>17</v>
+      </c>
+      <c r="G22">
+        <v>17</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>17</v>
+      </c>
+      <c r="J22">
+        <v>17</v>
+      </c>
+      <c r="K22">
+        <v>17</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <v>17</v>
+      </c>
+      <c r="N22">
+        <v>17</v>
+      </c>
+      <c r="O22">
+        <v>17</v>
+      </c>
+      <c r="P22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:16">
+      <c r="B23">
+        <v>20</v>
+      </c>
+      <c r="D23">
+        <v>88</v>
+      </c>
+      <c r="E23">
+        <v>11</v>
+      </c>
+      <c r="F23">
+        <v>11</v>
+      </c>
+      <c r="G23">
+        <v>10</v>
+      </c>
+      <c r="H23">
+        <v>0.02</v>
+      </c>
+      <c r="I23">
+        <v>10</v>
+      </c>
+      <c r="J23">
+        <v>4</v>
+      </c>
+      <c r="K23">
+        <v>11</v>
+      </c>
+      <c r="L23">
+        <v>0.15</v>
+      </c>
+      <c r="M23">
+        <v>11</v>
+      </c>
+      <c r="N23">
+        <v>11</v>
+      </c>
+      <c r="O23">
+        <v>11</v>
+      </c>
+      <c r="P23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:16">
+      <c r="B24">
+        <v>21</v>
+      </c>
+      <c r="D24">
+        <v>221</v>
+      </c>
+      <c r="E24">
+        <v>2</v>
+      </c>
+      <c r="F24">
+        <v>2</v>
+      </c>
+      <c r="G24">
+        <v>2</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>2</v>
+      </c>
+      <c r="J24">
+        <v>2</v>
+      </c>
+      <c r="K24">
+        <v>2</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <v>2</v>
+      </c>
+      <c r="N24">
+        <v>2</v>
+      </c>
+      <c r="O24">
+        <v>2</v>
+      </c>
+      <c r="P24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:16">
+      <c r="B25">
+        <v>22</v>
+      </c>
+      <c r="D25">
+        <v>2146</v>
+      </c>
+      <c r="E25">
+        <v>13</v>
+      </c>
+      <c r="F25">
+        <v>17</v>
+      </c>
+      <c r="G25">
+        <v>7</v>
+      </c>
+      <c r="H25">
+        <v>0.15</v>
+      </c>
+      <c r="I25">
+        <v>12</v>
+      </c>
+      <c r="J25">
+        <v>14</v>
+      </c>
+      <c r="K25">
+        <v>4</v>
+      </c>
+      <c r="L25">
+        <v>0.15</v>
+      </c>
+      <c r="M25">
+        <v>14</v>
+      </c>
+      <c r="N25">
+        <v>16</v>
+      </c>
+      <c r="O25">
+        <v>11</v>
+      </c>
+      <c r="P25">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="2:16">
+      <c r="B26">
+        <v>23</v>
+      </c>
+      <c r="D26">
+        <v>71</v>
+      </c>
+      <c r="E26">
+        <v>2</v>
+      </c>
+      <c r="F26">
+        <v>2</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+      <c r="H26">
+        <v>0.13</v>
+      </c>
+      <c r="I26">
+        <v>2</v>
+      </c>
+      <c r="J26">
+        <v>2</v>
+      </c>
+      <c r="K26">
+        <v>1</v>
+      </c>
+      <c r="L26">
+        <v>0.09</v>
+      </c>
+      <c r="M26">
+        <v>2</v>
+      </c>
+      <c r="N26">
+        <v>2</v>
+      </c>
+      <c r="O26">
+        <v>2</v>
+      </c>
+      <c r="P26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:16">
+      <c r="B27">
+        <v>24</v>
+      </c>
+      <c r="D27">
+        <v>313</v>
+      </c>
+      <c r="E27">
+        <v>4</v>
+      </c>
+      <c r="F27">
+        <v>4</v>
+      </c>
+      <c r="G27">
+        <v>4</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>4</v>
+      </c>
+      <c r="J27">
+        <v>4</v>
+      </c>
+      <c r="K27">
+        <v>4</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <v>4</v>
+      </c>
+      <c r="N27">
+        <v>4</v>
+      </c>
+      <c r="O27">
+        <v>4</v>
+      </c>
+      <c r="P27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:16">
+      <c r="B28">
+        <v>25</v>
+      </c>
+      <c r="D28">
+        <v>234</v>
+      </c>
+      <c r="E28">
+        <v>4</v>
+      </c>
+      <c r="F28">
+        <v>4</v>
+      </c>
+      <c r="G28">
+        <v>4</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <v>4</v>
+      </c>
+      <c r="J28">
+        <v>4</v>
+      </c>
+      <c r="K28">
+        <v>4</v>
+      </c>
+      <c r="L28">
+        <v>0</v>
+      </c>
+      <c r="M28">
+        <v>4</v>
+      </c>
+      <c r="N28">
+        <v>4</v>
+      </c>
+      <c r="O28">
+        <v>4</v>
+      </c>
+      <c r="P28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:16">
+      <c r="B29">
+        <v>26</v>
+      </c>
+      <c r="D29">
+        <v>245</v>
+      </c>
+      <c r="E29">
+        <v>8</v>
+      </c>
+      <c r="F29">
+        <v>8</v>
+      </c>
+      <c r="G29">
+        <v>8</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <v>8</v>
+      </c>
+      <c r="J29">
+        <v>8</v>
+      </c>
+      <c r="K29">
+        <v>8</v>
+      </c>
+      <c r="L29">
+        <v>0</v>
+      </c>
+      <c r="M29">
+        <v>8</v>
+      </c>
+      <c r="N29">
+        <v>8</v>
+      </c>
+      <c r="O29">
+        <v>8</v>
+      </c>
+      <c r="P29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:16">
+      <c r="B30">
+        <v>27</v>
+      </c>
+      <c r="D30">
+        <v>513</v>
+      </c>
+      <c r="E30">
+        <v>3</v>
+      </c>
+      <c r="F30">
+        <v>2</v>
+      </c>
+      <c r="G30">
+        <v>2</v>
+      </c>
+      <c r="H30">
+        <v>0.23</v>
+      </c>
+      <c r="I30">
+        <v>4</v>
+      </c>
+      <c r="J30">
+        <v>4</v>
+      </c>
+      <c r="K30">
+        <v>3</v>
+      </c>
+      <c r="L30">
+        <v>0.06</v>
+      </c>
+      <c r="M30">
+        <v>4</v>
+      </c>
+      <c r="N30">
+        <v>4</v>
+      </c>
+      <c r="O30">
+        <v>3</v>
+      </c>
+      <c r="P30">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="31" spans="2:16">
+      <c r="B31">
+        <v>28</v>
+      </c>
+      <c r="D31">
+        <v>645</v>
+      </c>
+      <c r="E31">
+        <v>8</v>
+      </c>
+      <c r="F31">
+        <v>8</v>
+      </c>
+      <c r="G31">
+        <v>6</v>
+      </c>
+      <c r="H31">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="I31">
+        <v>8</v>
+      </c>
+      <c r="J31">
+        <v>8</v>
+      </c>
+      <c r="K31">
+        <v>7</v>
+      </c>
+      <c r="L31">
+        <v>0.04</v>
+      </c>
+      <c r="M31">
+        <v>8</v>
+      </c>
+      <c r="N31">
+        <v>8</v>
+      </c>
+      <c r="O31">
+        <v>7</v>
+      </c>
+      <c r="P31">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="32" spans="2:16">
+      <c r="B32">
+        <v>29</v>
+      </c>
+      <c r="D32">
+        <v>1718</v>
+      </c>
+      <c r="E32">
+        <v>5</v>
+      </c>
+      <c r="F32">
+        <v>6</v>
+      </c>
+      <c r="G32">
+        <v>4</v>
+      </c>
+      <c r="H32">
+        <v>0.11</v>
+      </c>
+      <c r="I32">
+        <v>6</v>
+      </c>
+      <c r="J32">
+        <v>6</v>
+      </c>
+      <c r="K32">
+        <v>4</v>
+      </c>
+      <c r="L32">
+        <v>0.1</v>
+      </c>
+      <c r="M32">
+        <v>6</v>
+      </c>
+      <c r="N32">
+        <v>6</v>
+      </c>
+      <c r="O32">
+        <v>5</v>
+      </c>
+      <c r="P32">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="33" spans="2:16">
+      <c r="B33">
+        <v>30</v>
+      </c>
+      <c r="D33">
+        <v>172</v>
+      </c>
+      <c r="E33">
+        <v>4</v>
+      </c>
+      <c r="F33">
+        <v>4</v>
+      </c>
+      <c r="G33">
+        <v>4</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="I33">
+        <v>4</v>
+      </c>
+      <c r="J33">
+        <v>4</v>
+      </c>
+      <c r="K33">
+        <v>4</v>
+      </c>
+      <c r="L33">
+        <v>0</v>
+      </c>
+      <c r="M33">
+        <v>4</v>
+      </c>
+      <c r="N33">
+        <v>4</v>
+      </c>
+      <c r="O33">
+        <v>4</v>
+      </c>
+      <c r="P33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:16">
+      <c r="B34">
+        <v>31</v>
+      </c>
+      <c r="D34">
+        <v>68</v>
+      </c>
+      <c r="E34">
+        <v>38</v>
+      </c>
+      <c r="F34">
+        <v>46</v>
+      </c>
+      <c r="G34">
+        <v>30</v>
+      </c>
+      <c r="H34">
+        <v>0.1</v>
+      </c>
+      <c r="I34">
+        <v>36</v>
+      </c>
+      <c r="J34">
+        <v>45</v>
+      </c>
+      <c r="K34">
+        <v>30</v>
+      </c>
+      <c r="L34">
+        <v>0.12</v>
+      </c>
+      <c r="M34">
+        <v>38</v>
+      </c>
+      <c r="N34">
+        <v>45</v>
+      </c>
+      <c r="O34">
+        <v>30</v>
+      </c>
+      <c r="P34">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="35" spans="2:16">
+      <c r="B35">
+        <v>32</v>
+      </c>
+      <c r="D35">
+        <v>208</v>
+      </c>
+      <c r="E35">
+        <v>28</v>
+      </c>
+      <c r="F35">
+        <v>29</v>
+      </c>
+      <c r="G35">
+        <v>26</v>
+      </c>
+      <c r="H35">
+        <v>0.03</v>
+      </c>
+      <c r="I35">
+        <v>28</v>
+      </c>
+      <c r="J35">
+        <v>29</v>
+      </c>
+      <c r="K35">
+        <v>26</v>
+      </c>
+      <c r="L35">
+        <v>0.04</v>
+      </c>
+      <c r="M35">
+        <v>28</v>
+      </c>
+      <c r="N35">
+        <v>29</v>
+      </c>
+      <c r="O35">
+        <v>26</v>
+      </c>
+      <c r="P35">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="36" spans="2:16">
+      <c r="B36">
+        <v>33</v>
+      </c>
+      <c r="D36">
+        <v>571</v>
+      </c>
+      <c r="E36">
+        <v>68</v>
+      </c>
+      <c r="F36">
+        <v>68</v>
+      </c>
+      <c r="G36">
+        <v>68</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="I36">
+        <v>68</v>
+      </c>
+      <c r="J36">
+        <v>68</v>
+      </c>
+      <c r="K36">
+        <v>68</v>
+      </c>
+      <c r="L36">
+        <v>0</v>
+      </c>
+      <c r="M36">
+        <v>68</v>
+      </c>
+      <c r="N36">
+        <v>68</v>
+      </c>
+      <c r="O36">
+        <v>68</v>
+      </c>
+      <c r="P36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="2:16">
+      <c r="B37">
+        <v>34</v>
+      </c>
+      <c r="D37">
+        <v>602</v>
+      </c>
+      <c r="E37">
+        <v>65</v>
+      </c>
+      <c r="F37">
+        <v>65</v>
+      </c>
+      <c r="G37">
+        <v>65</v>
+      </c>
+      <c r="H37">
+        <v>0</v>
+      </c>
+      <c r="I37">
+        <v>65</v>
+      </c>
+      <c r="J37">
+        <v>65</v>
+      </c>
+      <c r="K37">
+        <v>65</v>
+      </c>
+      <c r="L37">
+        <v>0</v>
+      </c>
+      <c r="M37">
+        <v>65</v>
+      </c>
+      <c r="N37">
+        <v>65</v>
+      </c>
+      <c r="O37">
+        <v>65</v>
+      </c>
+      <c r="P37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="2:16">
+      <c r="B38">
+        <v>35</v>
+      </c>
+      <c r="D38">
+        <v>162</v>
+      </c>
+      <c r="E38">
+        <v>36</v>
+      </c>
+      <c r="F38">
+        <v>36</v>
+      </c>
+      <c r="G38">
+        <v>36</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="I38">
+        <v>36</v>
+      </c>
+      <c r="J38">
+        <v>36</v>
+      </c>
+      <c r="K38">
+        <v>36</v>
+      </c>
+      <c r="L38">
+        <v>0</v>
+      </c>
+      <c r="M38">
+        <v>36</v>
+      </c>
+      <c r="N38">
+        <v>36</v>
+      </c>
+      <c r="O38">
+        <v>36</v>
+      </c>
+      <c r="P38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="2:16">
+      <c r="B39">
+        <v>36</v>
+      </c>
+      <c r="D39">
+        <v>470</v>
+      </c>
+      <c r="E39">
+        <v>65</v>
+      </c>
+      <c r="F39">
+        <v>71</v>
+      </c>
+      <c r="G39">
+        <v>60</v>
+      </c>
+      <c r="H39">
+        <v>0.04</v>
+      </c>
+      <c r="I39">
+        <v>66</v>
+      </c>
+      <c r="J39">
+        <v>78</v>
+      </c>
+      <c r="K39">
+        <v>62</v>
+      </c>
+      <c r="L39">
+        <v>0.04</v>
+      </c>
+      <c r="M39">
+        <v>69</v>
+      </c>
+      <c r="N39">
+        <v>78</v>
+      </c>
+      <c r="O39">
+        <v>64</v>
+      </c>
+      <c r="P39">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="40" spans="2:16">
+      <c r="B40">
+        <v>37</v>
+      </c>
+      <c r="D40">
+        <v>63</v>
+      </c>
+      <c r="E40">
+        <v>31</v>
+      </c>
+      <c r="F40">
+        <v>31</v>
+      </c>
+      <c r="G40">
+        <v>31</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+      <c r="I40">
+        <v>40</v>
+      </c>
+      <c r="J40">
+        <v>40</v>
+      </c>
+      <c r="K40">
+        <v>40</v>
+      </c>
+      <c r="L40">
+        <v>0</v>
+      </c>
+      <c r="M40">
+        <v>40</v>
+      </c>
+      <c r="N40">
+        <v>40</v>
+      </c>
+      <c r="O40">
+        <v>40</v>
+      </c>
+      <c r="P40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:16">
+      <c r="B41">
+        <v>38</v>
+      </c>
+      <c r="D41">
+        <v>1069</v>
+      </c>
+      <c r="E41">
+        <v>7</v>
+      </c>
+      <c r="F41">
+        <v>7</v>
+      </c>
+      <c r="G41">
+        <v>7</v>
+      </c>
+      <c r="H41">
+        <v>0</v>
+      </c>
+      <c r="I41">
+        <v>7</v>
+      </c>
+      <c r="J41">
+        <v>7</v>
+      </c>
+      <c r="K41">
+        <v>7</v>
+      </c>
+      <c r="L41">
+        <v>0</v>
+      </c>
+      <c r="M41">
+        <v>7</v>
+      </c>
+      <c r="N41">
+        <v>7</v>
+      </c>
+      <c r="O41">
+        <v>7</v>
+      </c>
+      <c r="P41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="2:16">
+      <c r="B42">
+        <v>39</v>
+      </c>
+      <c r="D42">
+        <v>1564</v>
+      </c>
+      <c r="E42">
+        <v>4</v>
+      </c>
+      <c r="F42">
+        <v>4</v>
+      </c>
+      <c r="G42">
+        <v>4</v>
+      </c>
+      <c r="H42">
+        <v>0</v>
+      </c>
+      <c r="I42">
+        <v>4</v>
+      </c>
+      <c r="J42">
+        <v>4</v>
+      </c>
+      <c r="K42">
+        <v>4</v>
+      </c>
+      <c r="L42">
+        <v>0</v>
+      </c>
+      <c r="M42">
+        <v>4</v>
+      </c>
+      <c r="N42">
+        <v>4</v>
+      </c>
+      <c r="O42">
+        <v>4</v>
+      </c>
+      <c r="P42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="2:16">
+      <c r="B43">
+        <v>40</v>
+      </c>
+      <c r="D43">
+        <v>94</v>
+      </c>
+      <c r="E43">
+        <v>3</v>
+      </c>
+      <c r="F43">
+        <v>5</v>
+      </c>
+      <c r="G43">
+        <v>2</v>
+      </c>
+      <c r="H43">
+        <v>0.2</v>
+      </c>
+      <c r="I43">
+        <v>3</v>
+      </c>
+      <c r="J43">
+        <v>5</v>
+      </c>
+      <c r="K43">
+        <v>2</v>
+      </c>
+      <c r="L43">
+        <v>0.27</v>
+      </c>
+      <c r="M43">
+        <v>3</v>
+      </c>
+      <c r="N43">
+        <v>5</v>
+      </c>
+      <c r="O43">
+        <v>2</v>
+      </c>
+      <c r="P43">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="44" spans="2:16">
+      <c r="B44">
+        <v>41</v>
+      </c>
+      <c r="D44">
+        <v>1603</v>
+      </c>
+      <c r="E44">
+        <v>26</v>
+      </c>
+      <c r="F44">
+        <v>27</v>
+      </c>
+      <c r="G44">
+        <v>26</v>
+      </c>
+      <c r="H44">
+        <v>0.02</v>
+      </c>
+      <c r="I44">
+        <v>26</v>
+      </c>
+      <c r="J44">
+        <v>27</v>
+      </c>
+      <c r="K44">
+        <v>26</v>
+      </c>
+      <c r="L44">
+        <v>0.02</v>
+      </c>
+      <c r="M44">
+        <v>27</v>
+      </c>
+      <c r="N44">
+        <v>27</v>
+      </c>
+      <c r="O44">
+        <v>26</v>
+      </c>
+      <c r="P44">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="45" spans="2:16">
+      <c r="B45">
+        <v>42</v>
+      </c>
+      <c r="D45">
+        <v>431</v>
+      </c>
+      <c r="E45">
+        <v>3</v>
+      </c>
+      <c r="F45">
+        <v>3</v>
+      </c>
+      <c r="G45">
+        <v>3</v>
+      </c>
+      <c r="H45">
+        <v>0</v>
+      </c>
+      <c r="I45">
+        <v>3</v>
+      </c>
+      <c r="J45">
+        <v>3</v>
+      </c>
+      <c r="K45">
+        <v>3</v>
+      </c>
+      <c r="L45">
+        <v>0</v>
+      </c>
+      <c r="M45">
+        <v>3</v>
+      </c>
+      <c r="N45">
+        <v>3</v>
+      </c>
+      <c r="O45">
+        <v>3</v>
+      </c>
+      <c r="P45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="2:16">
+      <c r="B46">
+        <v>43</v>
+      </c>
+      <c r="D46">
+        <v>279</v>
+      </c>
+      <c r="E46">
+        <v>15</v>
+      </c>
+      <c r="F46">
+        <v>21</v>
+      </c>
+      <c r="G46">
+        <v>11</v>
+      </c>
+      <c r="H46">
+        <v>0.2</v>
+      </c>
+      <c r="I46">
+        <v>17</v>
+      </c>
+      <c r="J46">
+        <v>21</v>
+      </c>
+      <c r="K46">
+        <v>12</v>
+      </c>
+      <c r="L46">
+        <v>0.16</v>
+      </c>
+      <c r="M46">
+        <v>17</v>
+      </c>
+      <c r="N46">
+        <v>21</v>
+      </c>
+      <c r="O46">
+        <v>12</v>
+      </c>
+      <c r="P46">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="47" spans="2:16">
+      <c r="B47">
+        <v>44</v>
+      </c>
+      <c r="D47">
+        <v>47</v>
+      </c>
+      <c r="E47">
+        <v>2</v>
+      </c>
+      <c r="F47">
+        <v>2</v>
+      </c>
+      <c r="G47">
+        <v>1</v>
+      </c>
+      <c r="H47">
+        <v>0.09</v>
+      </c>
+      <c r="I47">
+        <v>3</v>
+      </c>
+      <c r="J47">
+        <v>3</v>
+      </c>
+      <c r="K47">
+        <v>2</v>
+      </c>
+      <c r="L47">
+        <v>0.06</v>
+      </c>
+      <c r="M47">
+        <v>3</v>
+      </c>
+      <c r="N47">
+        <v>3</v>
+      </c>
+      <c r="O47">
+        <v>3</v>
+      </c>
+      <c r="P47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="2:16">
+      <c r="B48">
+        <v>45</v>
+      </c>
+      <c r="D48">
+        <v>762</v>
+      </c>
+      <c r="E48">
+        <v>3</v>
+      </c>
+      <c r="F48">
+        <v>3</v>
+      </c>
+      <c r="G48">
+        <v>3</v>
+      </c>
+      <c r="H48">
+        <v>0</v>
+      </c>
+      <c r="I48">
+        <v>3</v>
+      </c>
+      <c r="J48">
+        <v>3</v>
+      </c>
+      <c r="K48">
+        <v>3</v>
+      </c>
+      <c r="L48">
+        <v>0</v>
+      </c>
+      <c r="M48">
+        <v>3</v>
+      </c>
+      <c r="N48">
+        <v>3</v>
+      </c>
+      <c r="O48">
+        <v>3</v>
+      </c>
+      <c r="P48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="2:16">
+      <c r="B49">
+        <v>46</v>
+      </c>
+      <c r="D49">
+        <v>491</v>
+      </c>
+      <c r="E49">
+        <v>16</v>
+      </c>
+      <c r="F49">
+        <v>17</v>
+      </c>
+      <c r="G49">
+        <v>12</v>
+      </c>
+      <c r="H49">
+        <v>0.08</v>
+      </c>
+      <c r="I49">
+        <v>23</v>
+      </c>
+      <c r="J49">
+        <v>25</v>
+      </c>
+      <c r="K49">
+        <v>22</v>
+      </c>
+      <c r="L49">
+        <v>0.03</v>
+      </c>
+      <c r="M49">
+        <v>24</v>
+      </c>
+      <c r="N49">
+        <v>25</v>
+      </c>
+      <c r="O49">
+        <v>22</v>
+      </c>
+      <c r="P49">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="50" spans="2:16">
+      <c r="B50">
+        <v>47</v>
+      </c>
+      <c r="D50">
+        <v>32</v>
+      </c>
+      <c r="E50">
+        <v>53</v>
+      </c>
+      <c r="F50">
+        <v>53</v>
+      </c>
+      <c r="G50">
+        <v>53</v>
+      </c>
+      <c r="H50">
+        <v>0</v>
+      </c>
+      <c r="I50">
+        <v>53</v>
+      </c>
+      <c r="J50">
+        <v>53</v>
+      </c>
+      <c r="K50">
+        <v>53</v>
+      </c>
+      <c r="L50">
+        <v>0</v>
+      </c>
+      <c r="M50">
+        <v>53</v>
+      </c>
+      <c r="N50">
+        <v>53</v>
+      </c>
+      <c r="O50">
+        <v>53</v>
+      </c>
+      <c r="P50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="2:16">
+      <c r="B51">
+        <v>48</v>
+      </c>
+      <c r="D51">
+        <v>332</v>
+      </c>
+      <c r="E51">
+        <v>7</v>
+      </c>
+      <c r="F51">
+        <v>8</v>
+      </c>
+      <c r="G51">
+        <v>7</v>
+      </c>
+      <c r="H51">
+        <v>0.03</v>
+      </c>
+      <c r="I51">
+        <v>7</v>
+      </c>
+      <c r="J51">
+        <v>8</v>
+      </c>
+      <c r="K51">
+        <v>6</v>
+      </c>
+      <c r="L51">
+        <v>0.08</v>
+      </c>
+      <c r="M51">
+        <v>8</v>
+      </c>
+      <c r="N51">
+        <v>8</v>
+      </c>
+      <c r="O51">
+        <v>7</v>
+      </c>
+      <c r="P51">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="52" spans="2:16">
+      <c r="B52">
+        <v>49</v>
+      </c>
+      <c r="D52">
+        <v>178</v>
+      </c>
+      <c r="E52">
+        <v>43</v>
+      </c>
+      <c r="F52">
+        <v>45</v>
+      </c>
+      <c r="G52">
+        <v>40</v>
+      </c>
+      <c r="H52">
+        <v>0.02</v>
+      </c>
+      <c r="I52">
+        <v>44</v>
+      </c>
+      <c r="J52">
+        <v>46</v>
+      </c>
+      <c r="K52">
+        <v>42</v>
+      </c>
+      <c r="L52">
+        <v>0.02</v>
+      </c>
+      <c r="M52">
+        <v>44</v>
+      </c>
+      <c r="N52">
+        <v>45</v>
+      </c>
+      <c r="O52">
+        <v>42</v>
+      </c>
+      <c r="P52">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="53" spans="2:16">
+      <c r="B53">
+        <v>50</v>
+      </c>
+      <c r="D53">
+        <v>119</v>
+      </c>
+      <c r="E53">
+        <v>19</v>
+      </c>
+      <c r="F53">
+        <v>19</v>
+      </c>
+      <c r="G53">
+        <v>19</v>
+      </c>
+      <c r="H53">
+        <v>0</v>
+      </c>
+      <c r="I53">
+        <v>19</v>
+      </c>
+      <c r="J53">
+        <v>19</v>
+      </c>
+      <c r="K53">
+        <v>19</v>
+      </c>
+      <c r="L53">
+        <v>0</v>
+      </c>
+      <c r="M53">
+        <v>19</v>
+      </c>
+      <c r="N53">
+        <v>19</v>
+      </c>
+      <c r="O53">
+        <v>19</v>
+      </c>
+      <c r="P53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="2:16">
+      <c r="B54">
+        <v>51</v>
+      </c>
+      <c r="D54">
+        <v>222</v>
+      </c>
+      <c r="E54">
+        <v>3</v>
+      </c>
+      <c r="F54">
+        <v>3</v>
+      </c>
+      <c r="G54">
+        <v>3</v>
+      </c>
+      <c r="H54">
+        <v>0</v>
+      </c>
+      <c r="I54">
+        <v>3</v>
+      </c>
+      <c r="J54">
+        <v>3</v>
+      </c>
+      <c r="K54">
+        <v>3</v>
+      </c>
+      <c r="L54">
+        <v>0</v>
+      </c>
+      <c r="M54">
+        <v>3</v>
+      </c>
+      <c r="N54">
+        <v>3</v>
+      </c>
+      <c r="O54">
+        <v>3</v>
+      </c>
+      <c r="P54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="2:16">
+      <c r="B55">
+        <v>52</v>
+      </c>
+      <c r="D55">
+        <v>460</v>
+      </c>
+      <c r="E55">
+        <v>21</v>
+      </c>
+      <c r="F55">
+        <v>22</v>
+      </c>
+      <c r="G55">
+        <v>21</v>
+      </c>
+      <c r="H55">
+        <v>0.02</v>
+      </c>
+      <c r="I55">
+        <v>21</v>
+      </c>
+      <c r="J55">
+        <v>22</v>
+      </c>
+      <c r="K55">
+        <v>21</v>
+      </c>
+      <c r="L55">
+        <v>0.01</v>
+      </c>
+      <c r="M55">
+        <v>21</v>
+      </c>
+      <c r="N55">
+        <v>22</v>
+      </c>
+      <c r="O55">
+        <v>21</v>
+      </c>
+      <c r="P55">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="56" spans="2:16">
+      <c r="B56">
+        <v>53</v>
+      </c>
+      <c r="D56">
+        <v>3970</v>
+      </c>
+      <c r="E56">
+        <v>5</v>
+      </c>
+      <c r="F56">
+        <v>5</v>
+      </c>
+      <c r="G56">
+        <v>5</v>
+      </c>
+      <c r="H56">
+        <v>0</v>
+      </c>
+      <c r="I56">
+        <v>5</v>
+      </c>
+      <c r="J56">
+        <v>5</v>
+      </c>
+      <c r="K56">
+        <v>5</v>
+      </c>
+      <c r="L56">
+        <v>0</v>
+      </c>
+      <c r="M56">
+        <v>5</v>
+      </c>
+      <c r="N56">
+        <v>5</v>
+      </c>
+      <c r="O56">
+        <v>5</v>
+      </c>
+      <c r="P56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="2:16">
+      <c r="B57">
+        <v>54</v>
+      </c>
+      <c r="D57">
+        <v>311</v>
+      </c>
+      <c r="E57">
+        <v>5</v>
+      </c>
+      <c r="F57">
+        <v>5</v>
+      </c>
+      <c r="G57">
+        <v>5</v>
+      </c>
+      <c r="H57">
+        <v>0</v>
+      </c>
+      <c r="I57">
+        <v>5</v>
+      </c>
+      <c r="J57">
+        <v>6</v>
+      </c>
+      <c r="K57">
+        <v>5</v>
+      </c>
+      <c r="L57">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="M57">
+        <v>5</v>
+      </c>
+      <c r="N57">
+        <v>7</v>
+      </c>
+      <c r="O57">
+        <v>5</v>
+      </c>
+      <c r="P57">
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="58" spans="2:16">
+      <c r="B58">
+        <v>55</v>
+      </c>
+      <c r="D58">
+        <v>277</v>
+      </c>
+      <c r="E58">
+        <v>8</v>
+      </c>
+      <c r="F58">
+        <v>8</v>
+      </c>
+      <c r="G58">
+        <v>8</v>
+      </c>
+      <c r="H58">
+        <v>0</v>
+      </c>
+      <c r="I58">
+        <v>8</v>
+      </c>
+      <c r="J58">
+        <v>8</v>
+      </c>
+      <c r="K58">
+        <v>8</v>
+      </c>
+      <c r="L58">
+        <v>0</v>
+      </c>
+      <c r="M58">
+        <v>8</v>
+      </c>
+      <c r="N58">
+        <v>8</v>
+      </c>
+      <c r="O58">
+        <v>8</v>
+      </c>
+      <c r="P58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="2:16">
+      <c r="B59">
+        <v>56</v>
+      </c>
+      <c r="D59">
+        <v>1031</v>
+      </c>
+      <c r="E59">
+        <v>13</v>
+      </c>
+      <c r="F59">
+        <v>13</v>
+      </c>
+      <c r="G59">
+        <v>13</v>
+      </c>
+      <c r="H59">
+        <v>0</v>
+      </c>
+      <c r="I59">
+        <v>13</v>
+      </c>
+      <c r="J59">
+        <v>13</v>
+      </c>
+      <c r="K59">
+        <v>13</v>
+      </c>
+      <c r="L59">
+        <v>0</v>
+      </c>
+      <c r="M59">
+        <v>13</v>
+      </c>
+      <c r="N59">
+        <v>13</v>
+      </c>
+      <c r="O59">
+        <v>13</v>
+      </c>
+      <c r="P59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="2:16">
+      <c r="B60">
+        <v>57</v>
+      </c>
+      <c r="D60">
+        <v>763</v>
+      </c>
+      <c r="E60">
+        <v>17</v>
+      </c>
+      <c r="F60">
+        <v>17</v>
+      </c>
+      <c r="G60">
+        <v>17</v>
+      </c>
+      <c r="H60">
+        <v>0.01</v>
+      </c>
+      <c r="I60">
+        <v>17</v>
+      </c>
+      <c r="J60">
+        <v>17</v>
+      </c>
+      <c r="K60">
+        <v>16</v>
+      </c>
+      <c r="L60">
+        <v>0.01</v>
+      </c>
+      <c r="M60">
+        <v>17</v>
+      </c>
+      <c r="N60">
+        <v>17</v>
+      </c>
+      <c r="O60">
+        <v>17</v>
+      </c>
+      <c r="P60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="2:16">
+      <c r="B61">
+        <v>58</v>
+      </c>
+      <c r="D61">
+        <v>445</v>
+      </c>
+      <c r="E61">
+        <v>12</v>
+      </c>
+      <c r="F61">
+        <v>12</v>
+      </c>
+      <c r="G61">
+        <v>12</v>
+      </c>
+      <c r="H61">
+        <v>0</v>
+      </c>
+      <c r="I61">
+        <v>12</v>
+      </c>
+      <c r="J61">
+        <v>12</v>
+      </c>
+      <c r="K61">
+        <v>12</v>
+      </c>
+      <c r="L61">
+        <v>0</v>
+      </c>
+      <c r="M61">
+        <v>12</v>
+      </c>
+      <c r="N61">
+        <v>12</v>
+      </c>
+      <c r="O61">
+        <v>12</v>
+      </c>
+      <c r="P61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="2:16">
+      <c r="B62">
+        <v>59</v>
+      </c>
+      <c r="D62">
+        <v>318</v>
+      </c>
+      <c r="E62">
+        <v>19</v>
+      </c>
+      <c r="F62">
+        <v>9</v>
+      </c>
+      <c r="G62">
+        <v>19</v>
+      </c>
+      <c r="H62">
+        <v>0</v>
+      </c>
+      <c r="I62">
+        <v>19</v>
+      </c>
+      <c r="J62">
+        <v>19</v>
+      </c>
+      <c r="K62">
+        <v>19</v>
+      </c>
+      <c r="L62">
+        <v>0</v>
+      </c>
+      <c r="M62">
+        <v>19</v>
+      </c>
+      <c r="N62">
+        <v>19</v>
+      </c>
+      <c r="O62">
+        <v>19</v>
+      </c>
+      <c r="P62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="2:16">
+      <c r="B63">
+        <v>60</v>
+      </c>
+      <c r="D63">
+        <v>546</v>
+      </c>
+      <c r="E63">
+        <v>23</v>
+      </c>
+      <c r="F63">
+        <v>21</v>
+      </c>
+      <c r="G63">
+        <v>21</v>
+      </c>
+      <c r="H63">
+        <v>0.04</v>
+      </c>
+      <c r="I63">
+        <v>23</v>
+      </c>
+      <c r="J63">
+        <v>24</v>
+      </c>
+      <c r="K63">
+        <v>23</v>
+      </c>
+      <c r="L63">
+        <v>0.02</v>
+      </c>
+      <c r="M63">
+        <v>24</v>
+      </c>
+      <c r="N63">
+        <v>24</v>
+      </c>
+      <c r="O63">
+        <v>23</v>
+      </c>
+      <c r="P63">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="64" spans="2:16">
+      <c r="D64" s="16">
+        <f>SUM(D4:D63)</f>
+        <v>35785</v>
+      </c>
+      <c r="E64" s="25">
+        <f>SUM(E4:E63)</f>
+        <v>1040</v>
+      </c>
+      <c r="F64">
+        <f t="shared" ref="F64:P64" si="0">SUM(F4:F63)</f>
+        <v>1075</v>
+      </c>
+      <c r="G64">
+        <f t="shared" si="0"/>
+        <v>973</v>
+      </c>
+      <c r="H64">
+        <f t="shared" si="0"/>
+        <v>2.42</v>
+      </c>
+      <c r="I64" s="26">
+        <f t="shared" si="0"/>
+        <v>1061</v>
+      </c>
+      <c r="J64" s="26">
+        <f t="shared" si="0"/>
+        <v>1106</v>
+      </c>
+      <c r="K64">
+        <f t="shared" si="0"/>
+        <v>1009</v>
+      </c>
+      <c r="L64">
+        <f t="shared" si="0"/>
+        <v>2.3499999999999996</v>
+      </c>
+      <c r="M64" s="26">
+        <f t="shared" si="0"/>
+        <v>1075</v>
+      </c>
+      <c r="N64" s="25">
+        <f t="shared" si="0"/>
+        <v>1118</v>
+      </c>
+      <c r="O64" s="25">
+        <f t="shared" si="0"/>
+        <v>1032</v>
+      </c>
+      <c r="P64">
+        <f t="shared" si="0"/>
+        <v>1.8200000000000003</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="N2:O2"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -35124,6 +38112,23 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet71.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">

</xml_diff>

<commit_message>
some very minor changes made.
</commit_message>
<xml_diff>
--- a/papers/ISSTA_DSSR/60classes.xlsx
+++ b/papers/ISSTA_DSSR/60classes.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22220"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="22020" tabRatio="863" firstSheet="54" activeTab="60"/>
+    <workbookView xWindow="28800" yWindow="-440" windowWidth="25600" windowHeight="20480" tabRatio="863" firstSheet="54" activeTab="62"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -69,7 +69,7 @@
     <sheet name="Sheet60" sheetId="60" r:id="rId60"/>
     <sheet name="T-test results" sheetId="75" r:id="rId61"/>
     <sheet name="as in paper" sheetId="77" r:id="rId62"/>
-    <sheet name="Sheet64" sheetId="64" r:id="rId63"/>
+    <sheet name="Graph" sheetId="64" r:id="rId63"/>
     <sheet name="Sheet65" sheetId="65" r:id="rId64"/>
     <sheet name="Sheet66" sheetId="66" r:id="rId65"/>
     <sheet name="Sheet67" sheetId="67" r:id="rId66"/>
@@ -89,7 +89,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2565" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2605" uniqueCount="138">
   <si>
     <t>org.antlr.grammar.v3.ActionTranslator</t>
   </si>
@@ -492,6 +492,18 @@
   <si>
     <t>R. Std</t>
   </si>
+  <si>
+    <t>DSSr</t>
+  </si>
+  <si>
+    <t>DSSR over R</t>
+  </si>
+  <si>
+    <t>DSSR over R+</t>
+  </si>
+  <si>
+    <t>R+ over R</t>
+  </si>
 </sst>
 </file>
 
@@ -503,7 +515,14 @@
     <numFmt numFmtId="166" formatCode="0.00000000"/>
     <numFmt numFmtId="167" formatCode="0.000000000"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -624,341 +643,370 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="321">
+  <cellStyleXfs count="350">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -968,25 +1016,30 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="321" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="321">
+  <cellStyles count="350">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1147,6 +1200,20 @@
     <cellStyle name="Followed Hyperlink" xfId="316" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="318" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="320" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="323" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="325" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="327" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="329" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="331" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="333" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="335" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="337" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="339" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="341" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="343" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="345" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="347" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="349" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1307,7 +1374,22 @@
     <cellStyle name="Hyperlink" xfId="315" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="317" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="319" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="322" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="324" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="326" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="328" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="330" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="332" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="334" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="336" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="338" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="340" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="342" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="344" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="346" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="348" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="321" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -33700,8 +33782,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G64" sqref="G64"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C29" sqref="C29:F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -33823,12 +33905,12 @@
       <c r="F8">
         <v>0.56000000000000005</v>
       </c>
-      <c r="I8" s="19" t="s">
+      <c r="I8" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="J8" s="19"/>
-      <c r="K8" s="19"/>
-      <c r="L8" s="19"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="24"/>
+      <c r="L8" s="24"/>
     </row>
     <row r="9" spans="2:12">
       <c r="B9" s="15">
@@ -33849,10 +33931,10 @@
       <c r="G9" t="s">
         <v>118</v>
       </c>
-      <c r="I9" s="19"/>
-      <c r="J9" s="19"/>
-      <c r="K9" s="19"/>
-      <c r="L9" s="19"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="24"/>
+      <c r="L9" s="24"/>
     </row>
     <row r="10" spans="2:12">
       <c r="B10" s="15">
@@ -33861,10 +33943,10 @@
       <c r="C10" t="s">
         <v>82</v>
       </c>
-      <c r="I10" s="19"/>
-      <c r="J10" s="19"/>
-      <c r="K10" s="19"/>
-      <c r="L10" s="19"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="24"/>
+      <c r="L10" s="24"/>
     </row>
     <row r="11" spans="2:12">
       <c r="B11" s="15">
@@ -33882,10 +33964,10 @@
       <c r="F11">
         <v>0.13</v>
       </c>
-      <c r="I11" s="19"/>
-      <c r="J11" s="19"/>
-      <c r="K11" s="19"/>
-      <c r="L11" s="19"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="24"/>
+      <c r="L11" s="24"/>
     </row>
     <row r="12" spans="2:12">
       <c r="B12" s="15">
@@ -33911,12 +33993,12 @@
       <c r="F13">
         <v>0.3</v>
       </c>
-      <c r="I13" s="19" t="s">
+      <c r="I13" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="J13" s="19"/>
-      <c r="K13" s="19"/>
-      <c r="L13" s="19"/>
+      <c r="J13" s="24"/>
+      <c r="K13" s="24"/>
+      <c r="L13" s="24"/>
     </row>
     <row r="14" spans="2:12">
       <c r="B14" s="15">
@@ -33925,10 +34007,10 @@
       <c r="C14" t="s">
         <v>86</v>
       </c>
-      <c r="I14" s="19"/>
-      <c r="J14" s="19"/>
-      <c r="K14" s="19"/>
-      <c r="L14" s="19"/>
+      <c r="I14" s="24"/>
+      <c r="J14" s="24"/>
+      <c r="K14" s="24"/>
+      <c r="L14" s="24"/>
     </row>
     <row r="15" spans="2:12">
       <c r="B15" s="15">
@@ -33937,10 +34019,10 @@
       <c r="C15" t="s">
         <v>87</v>
       </c>
-      <c r="I15" s="19"/>
-      <c r="J15" s="19"/>
-      <c r="K15" s="19"/>
-      <c r="L15" s="19"/>
+      <c r="I15" s="24"/>
+      <c r="J15" s="24"/>
+      <c r="K15" s="24"/>
+      <c r="L15" s="24"/>
     </row>
     <row r="16" spans="2:12">
       <c r="B16" s="15">
@@ -33974,12 +34056,12 @@
       <c r="F18">
         <v>1</v>
       </c>
-      <c r="I18" s="19" t="s">
+      <c r="I18" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="J18" s="19"/>
-      <c r="K18" s="19"/>
-      <c r="L18" s="19"/>
+      <c r="J18" s="24"/>
+      <c r="K18" s="24"/>
+      <c r="L18" s="24"/>
     </row>
     <row r="19" spans="2:12">
       <c r="B19" s="15">
@@ -33988,10 +34070,10 @@
       <c r="C19" t="s">
         <v>92</v>
       </c>
-      <c r="I19" s="19"/>
-      <c r="J19" s="19"/>
-      <c r="K19" s="19"/>
-      <c r="L19" s="19"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
+      <c r="K19" s="24"/>
+      <c r="L19" s="24"/>
     </row>
     <row r="20" spans="2:12">
       <c r="B20" s="15">
@@ -34000,10 +34082,10 @@
       <c r="C20" t="s">
         <v>93</v>
       </c>
-      <c r="I20" s="19"/>
-      <c r="J20" s="19"/>
-      <c r="K20" s="19"/>
-      <c r="L20" s="19"/>
+      <c r="I20" s="24"/>
+      <c r="J20" s="24"/>
+      <c r="K20" s="24"/>
+      <c r="L20" s="24"/>
     </row>
     <row r="21" spans="2:12">
       <c r="B21" s="15">
@@ -34620,8 +34702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:P64"/>
   <sheetViews>
-    <sheetView topLeftCell="E10" workbookViewId="0">
-      <selection activeCell="P51" sqref="P51"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J42" sqref="J42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -34631,72 +34713,72 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:16">
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="25" t="s">
         <v>126</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="25" t="s">
         <v>127</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="25" t="s">
         <v>128</v>
       </c>
-      <c r="E2" s="21"/>
-      <c r="F2" s="22" t="s">
+      <c r="E2" s="19"/>
+      <c r="F2" s="26" t="s">
         <v>129</v>
       </c>
-      <c r="G2" s="22"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="23" t="s">
+      <c r="G2" s="26"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="27" t="s">
         <v>130</v>
       </c>
-      <c r="J2" s="23"/>
-      <c r="K2" s="24"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="24"/>
-      <c r="N2" s="23" t="s">
+      <c r="J2" s="27"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21"/>
+      <c r="N2" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="O2" s="23"/>
-      <c r="P2" s="24"/>
+      <c r="O2" s="27"/>
+      <c r="P2" s="21"/>
     </row>
     <row r="3" spans="2:16">
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="21" t="s">
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="F3" s="19" t="s">
         <v>131</v>
       </c>
-      <c r="G3" s="21" t="s">
+      <c r="G3" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="H3" s="21" t="s">
+      <c r="H3" s="19" t="s">
         <v>133</v>
       </c>
-      <c r="I3" s="24" t="s">
+      <c r="I3" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="J3" s="24" t="s">
+      <c r="J3" s="21" t="s">
         <v>131</v>
       </c>
-      <c r="K3" s="24" t="s">
+      <c r="K3" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="L3" s="24" t="s">
+      <c r="L3" s="21" t="s">
         <v>133</v>
       </c>
-      <c r="M3" s="24" t="s">
+      <c r="M3" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="N3" s="24" t="s">
+      <c r="N3" s="21" t="s">
         <v>131</v>
       </c>
-      <c r="O3" s="24" t="s">
+      <c r="O3" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="P3" s="24" t="s">
+      <c r="P3" s="21" t="s">
         <v>133</v>
       </c>
     </row>
@@ -37346,7 +37428,7 @@
         <f>SUM(D4:D63)</f>
         <v>35785</v>
       </c>
-      <c r="E64" s="25">
+      <c r="E64" s="22">
         <f>SUM(E4:E63)</f>
         <v>1040</v>
       </c>
@@ -37362,11 +37444,11 @@
         <f t="shared" si="0"/>
         <v>2.42</v>
       </c>
-      <c r="I64" s="26">
+      <c r="I64" s="23">
         <f t="shared" si="0"/>
         <v>1061</v>
       </c>
-      <c r="J64" s="26">
+      <c r="J64" s="23">
         <f t="shared" si="0"/>
         <v>1106</v>
       </c>
@@ -37378,15 +37460,15 @@
         <f t="shared" si="0"/>
         <v>2.3499999999999996</v>
       </c>
-      <c r="M64" s="26">
+      <c r="M64" s="23">
         <f t="shared" si="0"/>
         <v>1075</v>
       </c>
-      <c r="N64" s="25">
+      <c r="N64" s="22">
         <f t="shared" si="0"/>
         <v>1118</v>
       </c>
-      <c r="O64" s="25">
+      <c r="O64" s="22">
         <f t="shared" si="0"/>
         <v>1032</v>
       </c>
@@ -37397,12 +37479,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="N2:O2"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="I2:J2"/>
-    <mergeCell ref="N2:O2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -37416,13 +37498,909 @@
 
 <file path=xl/worksheets/sheet63.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B2:J33"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4:J32"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="16.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:10">
+      <c r="B2" s="25" t="s">
+        <v>126</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>127</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10">
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="F3" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="H3" t="s">
+        <v>135</v>
+      </c>
+      <c r="I3" t="s">
+        <v>136</v>
+      </c>
+      <c r="J3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>80</v>
+      </c>
+      <c r="E4">
+        <v>80</v>
+      </c>
+      <c r="F4">
+        <v>80</v>
+      </c>
+      <c r="H4" s="29">
+        <f>(F4-D4)/D4</f>
+        <v>0</v>
+      </c>
+      <c r="I4" s="29">
+        <f>((F4-D4)/D4)</f>
+        <v>0</v>
+      </c>
+      <c r="J4" s="29">
+        <f>((F4-E4)/E4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10">
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="H5" s="29">
+        <f t="shared" ref="H5:H32" si="0">(F5-D5)/D5</f>
+        <v>0</v>
+      </c>
+      <c r="I5" s="29">
+        <f t="shared" ref="I5:I32" si="1">((F5-D5)/D5)</f>
+        <v>0</v>
+      </c>
+      <c r="J5" s="29">
+        <f t="shared" ref="J5:J32" si="2">((F5-E5)/E5)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10">
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>7</v>
+      </c>
+      <c r="E6">
+        <v>6</v>
+      </c>
+      <c r="F6">
+        <v>7</v>
+      </c>
+      <c r="H6" s="29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I6" s="29">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J6" s="29">
+        <f t="shared" si="2"/>
+        <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10">
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
+      <c r="H7" s="29">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="I7" s="29">
+        <f t="shared" si="1"/>
+        <v>0.25</v>
+      </c>
+      <c r="J7" s="29">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10">
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <v>33</v>
+      </c>
+      <c r="E8">
+        <v>35</v>
+      </c>
+      <c r="F8">
+        <v>36</v>
+      </c>
+      <c r="H8" s="29">
+        <f t="shared" si="0"/>
+        <v>9.0909090909090912E-2</v>
+      </c>
+      <c r="I8" s="29">
+        <f t="shared" si="1"/>
+        <v>9.0909090909090912E-2</v>
+      </c>
+      <c r="J8" s="29">
+        <f t="shared" si="2"/>
+        <v>2.8571428571428571E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10">
+      <c r="B9">
+        <v>6</v>
+      </c>
+      <c r="C9" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="D9">
+        <v>7</v>
+      </c>
+      <c r="E9">
+        <v>7</v>
+      </c>
+      <c r="F9">
+        <v>7</v>
+      </c>
+      <c r="H9" s="29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I9" s="29">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J9" s="29">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10">
+      <c r="B10">
+        <v>7</v>
+      </c>
+      <c r="C10" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10">
+        <v>8</v>
+      </c>
+      <c r="E10">
+        <v>8</v>
+      </c>
+      <c r="F10">
+        <v>8</v>
+      </c>
+      <c r="H10" s="29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I10" s="29">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J10" s="29">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10">
+      <c r="B11">
+        <v>8</v>
+      </c>
+      <c r="C11" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="D11">
+        <v>12</v>
+      </c>
+      <c r="E11">
+        <v>12</v>
+      </c>
+      <c r="F11">
+        <v>12</v>
+      </c>
+      <c r="H11" s="29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I11" s="29">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J11" s="29">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10">
+      <c r="B12">
+        <v>9</v>
+      </c>
+      <c r="C12" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="D12">
+        <v>11</v>
+      </c>
+      <c r="E12">
+        <v>10</v>
+      </c>
+      <c r="F12">
+        <v>11</v>
+      </c>
+      <c r="H12" s="29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I12" s="29">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J12" s="29">
+        <f t="shared" si="2"/>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10">
+      <c r="B13">
+        <v>10</v>
+      </c>
+      <c r="C13" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13">
+        <v>13</v>
+      </c>
+      <c r="E13">
+        <v>12</v>
+      </c>
+      <c r="F13">
+        <v>14</v>
+      </c>
+      <c r="H13" s="29">
+        <f t="shared" si="0"/>
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="I13" s="29">
+        <f t="shared" si="1"/>
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="J13" s="29">
+        <f t="shared" si="2"/>
+        <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10">
+      <c r="B14">
+        <v>11</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+      <c r="F14">
+        <v>2</v>
+      </c>
+      <c r="H14" s="29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I14" s="29">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J14" s="29">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10">
+      <c r="B15">
+        <v>12</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15">
+        <v>3</v>
+      </c>
+      <c r="E15">
+        <v>4</v>
+      </c>
+      <c r="F15">
+        <v>4</v>
+      </c>
+      <c r="H15" s="29">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I15" s="29">
+        <f t="shared" si="1"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="J15" s="29">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10">
+      <c r="B16">
+        <v>13</v>
+      </c>
+      <c r="C16" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="1">
+        <v>8</v>
+      </c>
+      <c r="E16" s="1">
+        <v>8</v>
+      </c>
+      <c r="F16" s="1">
+        <v>8</v>
+      </c>
+      <c r="H16" s="29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I16" s="29">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J16" s="29">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10">
+      <c r="B17">
+        <v>14</v>
+      </c>
+      <c r="C17" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17">
+        <v>5</v>
+      </c>
+      <c r="E17">
+        <v>6</v>
+      </c>
+      <c r="F17">
+        <v>6</v>
+      </c>
+      <c r="H17" s="29">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="I17" s="29">
+        <f t="shared" si="1"/>
+        <v>0.2</v>
+      </c>
+      <c r="J17" s="29">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10">
+      <c r="B18">
+        <v>15</v>
+      </c>
+      <c r="C18" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18">
+        <v>38</v>
+      </c>
+      <c r="E18">
+        <v>36</v>
+      </c>
+      <c r="F18">
+        <v>38</v>
+      </c>
+      <c r="H18" s="29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I18" s="29">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J18" s="29">
+        <f t="shared" si="2"/>
+        <v>5.5555555555555552E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10">
+      <c r="B19">
+        <v>16</v>
+      </c>
+      <c r="C19" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19">
+        <v>28</v>
+      </c>
+      <c r="E19">
+        <v>28</v>
+      </c>
+      <c r="F19">
+        <v>28</v>
+      </c>
+      <c r="H19" s="29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I19" s="29">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J19" s="29">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10">
+      <c r="B20">
+        <v>17</v>
+      </c>
+      <c r="C20" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20">
+        <v>65</v>
+      </c>
+      <c r="E20">
+        <v>66</v>
+      </c>
+      <c r="F20">
+        <v>69</v>
+      </c>
+      <c r="H20" s="29">
+        <f t="shared" si="0"/>
+        <v>6.1538461538461542E-2</v>
+      </c>
+      <c r="I20" s="29">
+        <f t="shared" si="1"/>
+        <v>6.1538461538461542E-2</v>
+      </c>
+      <c r="J20" s="29">
+        <f t="shared" si="2"/>
+        <v>4.5454545454545456E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10">
+      <c r="B21">
+        <v>18</v>
+      </c>
+      <c r="C21" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21">
+        <v>31</v>
+      </c>
+      <c r="E21">
+        <v>40</v>
+      </c>
+      <c r="F21">
+        <v>40</v>
+      </c>
+      <c r="H21" s="29">
+        <f t="shared" si="0"/>
+        <v>0.29032258064516131</v>
+      </c>
+      <c r="I21" s="29">
+        <f t="shared" si="1"/>
+        <v>0.29032258064516131</v>
+      </c>
+      <c r="J21" s="29">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10">
+      <c r="B22">
+        <v>19</v>
+      </c>
+      <c r="C22" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="D22">
+        <v>3</v>
+      </c>
+      <c r="E22">
+        <v>3</v>
+      </c>
+      <c r="F22">
+        <v>3</v>
+      </c>
+      <c r="H22" s="29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I22" s="29">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J22" s="29">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10">
+      <c r="B23">
+        <v>20</v>
+      </c>
+      <c r="C23" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="D23">
+        <v>26</v>
+      </c>
+      <c r="E23">
+        <v>26</v>
+      </c>
+      <c r="F23">
+        <v>27</v>
+      </c>
+      <c r="H23" s="29">
+        <f t="shared" si="0"/>
+        <v>3.8461538461538464E-2</v>
+      </c>
+      <c r="I23" s="29">
+        <f t="shared" si="1"/>
+        <v>3.8461538461538464E-2</v>
+      </c>
+      <c r="J23" s="29">
+        <f t="shared" si="2"/>
+        <v>3.8461538461538464E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10">
+      <c r="B24">
+        <v>21</v>
+      </c>
+      <c r="C24" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="D24">
+        <v>15</v>
+      </c>
+      <c r="E24">
+        <v>17</v>
+      </c>
+      <c r="F24">
+        <v>17</v>
+      </c>
+      <c r="H24" s="29">
+        <f t="shared" si="0"/>
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="I24" s="29">
+        <f t="shared" si="1"/>
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="J24" s="29">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10">
+      <c r="B25">
+        <v>22</v>
+      </c>
+      <c r="C25" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="D25">
+        <v>2</v>
+      </c>
+      <c r="E25">
+        <v>3</v>
+      </c>
+      <c r="F25">
+        <v>3</v>
+      </c>
+      <c r="H25" s="29">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="I25" s="29">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="J25" s="29">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10">
+      <c r="B26">
+        <v>23</v>
+      </c>
+      <c r="C26" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="D26">
+        <v>16</v>
+      </c>
+      <c r="E26">
+        <v>23</v>
+      </c>
+      <c r="F26">
+        <v>24</v>
+      </c>
+      <c r="H26" s="29">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="I26" s="29">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="J26" s="29">
+        <f t="shared" si="2"/>
+        <v>4.3478260869565216E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10">
+      <c r="B27">
+        <v>24</v>
+      </c>
+      <c r="C27" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="D27">
+        <v>7</v>
+      </c>
+      <c r="E27">
+        <v>7</v>
+      </c>
+      <c r="F27">
+        <v>8</v>
+      </c>
+      <c r="H27" s="29">
+        <f t="shared" si="0"/>
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="I27" s="29">
+        <f t="shared" si="1"/>
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="J27" s="29">
+        <f t="shared" si="2"/>
+        <v>0.14285714285714285</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10">
+      <c r="B28">
+        <v>25</v>
+      </c>
+      <c r="C28" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="D28">
+        <v>43</v>
+      </c>
+      <c r="E28">
+        <v>44</v>
+      </c>
+      <c r="F28">
+        <v>44</v>
+      </c>
+      <c r="H28" s="29">
+        <f t="shared" si="0"/>
+        <v>2.3255813953488372E-2</v>
+      </c>
+      <c r="I28" s="29">
+        <f t="shared" si="1"/>
+        <v>2.3255813953488372E-2</v>
+      </c>
+      <c r="J28" s="29">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10">
+      <c r="B29">
+        <v>26</v>
+      </c>
+      <c r="C29" s="23" t="s">
+        <v>112</v>
+      </c>
+      <c r="D29">
+        <v>21</v>
+      </c>
+      <c r="E29">
+        <v>21</v>
+      </c>
+      <c r="F29">
+        <v>21</v>
+      </c>
+      <c r="H29" s="29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I29" s="29">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J29" s="29">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10">
+      <c r="B30">
+        <v>27</v>
+      </c>
+      <c r="C30" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="D30">
+        <v>5</v>
+      </c>
+      <c r="E30">
+        <v>5</v>
+      </c>
+      <c r="F30">
+        <v>5</v>
+      </c>
+      <c r="H30" s="29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I30" s="29">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J30" s="29">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10">
+      <c r="B31">
+        <v>28</v>
+      </c>
+      <c r="C31" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="D31">
+        <v>17</v>
+      </c>
+      <c r="E31">
+        <v>17</v>
+      </c>
+      <c r="F31">
+        <v>17</v>
+      </c>
+      <c r="H31" s="29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I31" s="29">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J31" s="29">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10">
+      <c r="B32">
+        <v>29</v>
+      </c>
+      <c r="C32" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="D32">
+        <v>23</v>
+      </c>
+      <c r="E32">
+        <v>23</v>
+      </c>
+      <c r="F32">
+        <v>23</v>
+      </c>
+      <c r="H32" s="29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I32" s="29">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J32" s="29">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="4:6">
+      <c r="D33" s="22"/>
+      <c r="E33" s="23"/>
+      <c r="F33" s="23"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>